<commit_message>
feat: add excel reader
</commit_message>
<xml_diff>
--- a/sheets/1.xlsx
+++ b/sheets/1.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="76">
-  <si>
-    <t>Tarih (Yıl - Gün - Ay)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="75">
+  <si>
+    <t>Tarih (Yıl - Ay - Gün)</t>
   </si>
   <si>
     <t>Metin</t>
@@ -39,10 +39,7 @@
     <t>Yayın Yılı</t>
   </si>
   <si>
-    <t>İstisnai Durum</t>
-  </si>
-  <si>
-    <t>1215-21-R</t>
+    <t>1215-R-21</t>
   </si>
   <si>
     <t>Duhân, yevm'ül-isneyn</t>
@@ -60,7 +57,7 @@
     <t>Zeytinburnu Belediyesi Kültür Yayınları</t>
   </si>
   <si>
-    <t>1215-20-CA</t>
+    <t>1215-CA-20</t>
   </si>
   <si>
     <t>Çeharşenbe gicesi sâ'at birde Hasköyde ihrâk olunup bin aded mikdar re'âyâ hânesi yanmışdır.</t>
@@ -69,39 +66,42 @@
     <t>İstanbul, Hasköy</t>
   </si>
   <si>
-    <t xml:space="preserve">Martın on üçüncü Salı günü ve Şevvâlin otuzuncu günü
+    <t>?-?-?</t>
+  </si>
+  <si>
+    <t>Martın on üçüncü Salı günü ve Şevvâlin otuzuncu günü
 gicesi ve gündüzü şiddetli şitâ olup vâfir kar yağmışdır. Erba‘în kadar icrâ-yı hükm etmişdir
-</t>
-  </si>
-  <si>
-    <t>16. Harîk, der-Üsküdâr 15. Harîk, der-Galata 15. Harîk, der-Tekfûr Sarâyı 20. Ve Âhûrkapu ve Begoğlu 17. Azl-i Sekbanbaşı 19. Harîk-i (…) 20, der-Çifte Sarây</t>
+!!!-</t>
+  </si>
+  <si>
+    <t>16. Harîk, der-Üsküdâr 15. Harîk, der-Galata 15. Harîk, der-Tekfûr Sarâyı 20. Ve Âhûrkapu ve Begoğlu 17. Azl-i Sekbanbaşı 19. Harîk-i (…) 20, der-Çifte Sarây !!!-</t>
   </si>
   <si>
     <t>İstanbul; Üsküdar, Galata, Tekfur Sarayı, Ahırkapı, Beyoğlu, Çifte Saray</t>
   </si>
   <si>
-    <t>21. İbtida-i şiddet-i bârân 24, gâyet 27 evâ’il-i Eylül.</t>
-  </si>
-  <si>
-    <t>?-2-Şubat(Şevval)</t>
-  </si>
-  <si>
-    <t>Bâriden-i boran</t>
-  </si>
-  <si>
-    <t>?-21,23-Mart</t>
-  </si>
-  <si>
-    <t>Bâriden-i berf (Kar Soğuğu)</t>
-  </si>
-  <si>
-    <t>1216-26-Teşrin-I Evvel (Kasım ayının başı)</t>
-  </si>
-  <si>
-    <t>Dört gice donanma etdiler. Evvel gicesi, Pazar gicesi cebehâne edip sonra havâ müsâ‘ade etmeyip ertesi hefte Cum‘aertesi gicesi tersâne edip ve Pazar gicesi Humbarahâne edip ve yine havâ müsâ‘ade etmeyip Pazarertesi gicesi Tophâne de etmişdir</t>
-  </si>
-  <si>
-    <t>1228-27-Muharrem</t>
+    <t>21. İbtida-i şiddet-i bârân 24, gâyet 27 evâ’il-i Eylül. !!!-</t>
+  </si>
+  <si>
+    <t>?-L-2</t>
+  </si>
+  <si>
+    <t>Bâriden-i boran !!!-Şubat(Şevval)??? nasıl</t>
+  </si>
+  <si>
+    <t>1811-03-21</t>
+  </si>
+  <si>
+    <t>Bâriden-i berf (Kar Soğuğu) !!!-21,23-Mart .  --?-03-21</t>
+  </si>
+  <si>
+    <t>1216-09-26</t>
+  </si>
+  <si>
+    <t>Dört gice donanma etdiler. Evvel gicesi, Pazar gicesi cebehâne edip sonra havâ müsâ‘ade etmeyip ertesi hefte Cum‘aertesi gicesi tersâne edip ve Pazar gicesi Humbarahâne edip ve yine havâ müsâ‘ade etmeyip Pazarertesi gicesi Tophâne de etmişdir !!!-1216-26-Teşrin-I Evvel (Kasım ayının başı)</t>
+  </si>
+  <si>
+    <t>1228-M-27</t>
   </si>
   <si>
     <t xml:space="preserve">Âmeden-i miftâh-ı şerîf-i Medîne-i Münevvere, şerrefenallahu te’âlâ bi-şerefihâ ... Bu eyyâmda azîm şitâ olup ve bu alay-ı şerîf günü kar yağar idi. Ehl-i alayın üzerleri lâzım geldiği üzre karlı olup lâkin miftâh-ı şerîfin tahtında olan tepsi pûşîdesinin üzerinde kar
@@ -120,7 +120,7 @@
     <t xml:space="preserve">İstanbul; Zeytinburnu, Baruthane, Bahçekapısı </t>
   </si>
   <si>
-    <t>1228-6-S</t>
+    <t>1228-S-6</t>
   </si>
   <si>
     <t>İncimâd-ı bahr, der-pîş-i Fenâr ve Odunkapusu tâ karşu yaka</t>
@@ -129,26 +129,23 @@
     <t>İstanbul; Fener(?), Odunkapısı</t>
   </si>
   <si>
-    <t>1220?-?-?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edâ-yı namâz-ı Cum‘a, der-Câmi‘-i Selîmiye, der-Üsküdâr. Lâkin havâ muhâlif
+    <t>1220-?-?</t>
+  </si>
+  <si>
+    <t>Edâ-yı namâz-ı Cum‘a, der-Câmi‘-i Selîmiye, der-Üsküdâr. Lâkin havâ muhâlif
 olduğu içün pâdişâh-ı âlem-penâh namâza gitmemişdir.
-</t>
+!!!-</t>
   </si>
   <si>
     <t>İstanbul, Üsküdar</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Havâlar dahi güzel ve küşâd olduğundan derûnum dahi soğan zarı gibi kapanmış iken açıldı ve
+    <t>Havâlar dahi güzel ve küşâd olduğundan derûnum dahi soğan zarı gibi kapanmış iken açıldı ve
 âleme güzel sözler ile küşâyiş saçıldı 
-</t>
-  </si>
-  <si>
-    <t>1228-17-Muharrem</t>
+!!!-</t>
+  </si>
+  <si>
+    <t>1228-M-17</t>
   </si>
   <si>
     <t xml:space="preserve">İncimâd-ı kenâr-ı bahr, der-pîş-i Cebeali ve Fenâr
@@ -160,10 +157,10 @@
     <t>İstanbul; Cebeali, Fener(?)</t>
   </si>
   <si>
-    <t>1228 -18 Mart (Ra), 22 Rebî‘ü’l-evvel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Şitâ ve nüzûl-ı selc der-Mart, fî Ra sene 1228. Martın on sekizinci günü ve Rebî‘ü’l-evvelin
+    <t>1228-R-22</t>
+  </si>
+  <si>
+    <t>Şitâ ve nüzûl-ı selc der-Mart, fî Ra sene 1228. Martın on sekizinci günü ve Rebî‘ü’l-evvelin
 on altıncı Cum‘a günü bir mikdâr dolu yağıp ve bir mikdâr kar sepeleyip berd dahi ziyâde
 oldu. Cum‘aertesi gicesi sulu kar yağıp sabâhı iki parmağa karîb kar hâsıl olup ve ol gün
 erimeyip ba‘zı yerde cüz’î eseri kaldı. Ve dahi Pazar günü dahi soğuk olup gâh gâh kar sepeledi ve bugünlerde eberede rûzgârlar esmişdir ve dahi Pazarertesi günü ki gicesi ba‘zı
@@ -174,10 +171,10 @@
 eyyâmdan mukaddem eyyâmdan berü İstanbûl’da kömür fazla idi. Husûsan bu eyyâmda
 begâyet kalîl olup belki nâdir bulunur oldu. Ve muktezâ-yı vakt odun dahi ve sâ’ir me’kû-
 lâta dâir eşyâ dahi buna kıyâsdır
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1230 9 R </t>
+!!!-1228 -18 Mart (Ra), 22 Rebî‘ü’l-evvel</t>
+  </si>
+  <si>
+    <t>1230-9-R</t>
   </si>
   <si>
     <t xml:space="preserve">Zuhûr-ı şitâ ve nüzûl-ı selc, der-tâsi‘-i Mart ya‘nî rûz-ı tavîl, fî 9 R sene 1230, yevmü’sselâse. Gice dahi kar yağıp ferdâsı günü, Çehârşenbe günü ki nevrûz-ı sultânîdir. Dahi
@@ -186,7 +183,7 @@
 </t>
   </si>
   <si>
-    <t>1230 25 Temmuz (Ş)</t>
+    <t>1230-Ş-25</t>
   </si>
   <si>
     <t xml:space="preserve">Nüzûl-ı matar-ı kesîr ve zuhûr-ı seyl-i kesîr ve harâbkerdeniş-i ba‘zı mahal, selh-i Ş, sene
@@ -195,19 +192,19 @@
 </t>
   </si>
   <si>
-    <t>?-?-Ramazan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pazar gicesi ki Ramazân-ı şerîfin evvelki gicesidir, o kadar yağmur yağdı ki ba‘zı dîvârlar
+    <t>?-N-?</t>
+  </si>
+  <si>
+    <t>Pazar gicesi ki Ramazân-ı şerîfin evvelki gicesidir, o kadar yağmur yağdı ki ba‘zı dîvârlar
 sukûtundan başka azîm seyller zuhûr eyleyip ba‘zı mahallerde hâneler ve dekâkîn harâb
 edip Eyyûb semtinde seylde iki âdem helâk olduğu dahi mesmû‘dur.
-</t>
+!!!-</t>
   </si>
   <si>
     <t>İstanbul; Yenikapı, Eyüp</t>
   </si>
   <si>
-    <t>1231 23 Zi'l-hicce</t>
+    <t>1231-Z-23</t>
   </si>
   <si>
     <t xml:space="preserve">Zuhûr-ı alâmet ya‘nî kızıllık, der-âsumân, der-taraf-ı şimâlî. Sene 1231, Zi’l-hiccenin yigirmi üçüncü gicesi, Çehârşenbe gicesi cânib-i şimâlde şarkdan garba tûlânî bir kızıllık
@@ -219,7 +216,7 @@
 </t>
   </si>
   <si>
-    <t>1232 15 Ca.</t>
+    <t>1232-CA-15</t>
   </si>
   <si>
     <t xml:space="preserve">Zuhûr-ı harîk, der-Odahâ-yı Yeñiçeriyân ya‘nî, der-Yeñi Odalar, sene 1232. Der-şeb-i Çehârşenbe, fî 15 Ca. Çok mahalli muhterik olmuşdur; lâkin bi-hamdillahi te’âlâ etrâfına
@@ -231,7 +228,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1233 17 B</t>
+    <t xml:space="preserve"> 1233-B-17</t>
   </si>
   <si>
     <t xml:space="preserve">Zuhûr-ı furtına, fî hâdî aşere-i Mayıs, fî 17 B sene 1233, yevmü’s-sebt. Yevm-i mezbûrda
@@ -250,7 +247,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1235 17 Z </t>
+    <t>1235-Z-17</t>
   </si>
   <si>
     <t xml:space="preserve">Nüzûl-ı meges, ez-havâ, ez-ebr, fî 14 Z sene 1235, yevmü’l-Cum‘a, âşîr Eylül. İstanbûl’un
@@ -268,7 +265,7 @@
     <t>İstanbul; Çırpıcı Çayırı, Yeni Bahçe Çayırı</t>
   </si>
   <si>
-    <t xml:space="preserve">1236 5 M </t>
+    <t>1236-M-5</t>
   </si>
   <si>
     <t xml:space="preserve">Zuhûr-ı furtına-i azîm ve nüzûl-ı yah-çe-i kebîr [ü] kesîr, 5 M sene 1236, yevmü’l-ahad,
@@ -281,7 +278,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1245 9 M </t>
+    <t>1245-M-9</t>
   </si>
   <si>
     <t xml:space="preserve">Zuhûr-ı furtına-i azîm ve nüzûl-ı yah-çe-i kebîr ü kesîr, fî 9 M sene 1245, 29 Hazîrân fî
@@ -293,45 +290,45 @@
 </t>
   </si>
   <si>
-    <t>1338?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1338 senesi Cemâziye’l-evvelin 18’nci ve Şubat âhirinin 9’ncu Pazarertesi günü kar ya-
+    <t>1338-?-?</t>
+  </si>
+  <si>
+    <t>1338 senesi Cemâziye’l-evvelin 18’nci ve Şubat âhirinin 9’ncu Pazarertesi günü kar ya-
 ğarak iki karış mikdârı olmuşdur
-</t>
-  </si>
-  <si>
-    <t>1222 ? Ş</t>
-  </si>
-  <si>
-    <t>Tulû‘-ı Kuyruklu Yılduz, mâh-ı Ş sene 1222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1226 ? Receb </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tulû‘-ı necm-i acîb, der-mâh-ı Şa‘bân ve rivâyet-i ba‘z, der-mâh-ı Receb sene 1226. Mezkûr kevkeb, sâ’ir büyük yılduzlar mikdâr olup lâkin rengi kebûd ve revnak olup ve şarka
+!!!-</t>
+  </si>
+  <si>
+    <t>1222-Ş-?</t>
+  </si>
+  <si>
+    <t>Tulû‘-ı Kuyruklu Yılduz, mâh-ı Ş sene 1222 !!!-</t>
+  </si>
+  <si>
+    <t>1226-B-?</t>
+  </si>
+  <si>
+    <t>Tulû‘-ı necm-i acîb, der-mâh-ı Şa‘bân ve rivâyet-i ba‘z, der-mâh-ı Receb sene 1226. Mezkûr kevkeb, sâ’ir büyük yılduzlar mikdâr olup lâkin rengi kebûd ve revnak olup ve şarka
 mümted bir kulaç mikdârı ziyâsı olup ammâ evvel mümted olan ziyâsı ba‘zı gice bir mikdâr kasîr hattâ mehtâb oldukca azca olup garbîsi rü’yet olunur ve şimâli meyl ile şarkî
 seyri vardır. Müneccim-i sânî efendiden, mezkûr yılduz fenn-i nücûmda mücerrebü’lahkâm bir isim ile mevsûm yılduzlardan olmayıp alâyim kabîlindendir deyü mesmû‘dur.
 Ve bu târîh-i tahrîre dek mer’îdir. Her ne ise hayr bâd, 16 L, yevmü’s-sebt
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1233 15,29 C </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vukû‘-ı husûf-ı kamer, fî 15 C, leyletü’l-isneyn ve küsûf-ı şems, fî 29 C sene 1233,
+!!!-</t>
+  </si>
+  <si>
+    <t>1233-C-15</t>
+  </si>
+  <si>
+    <t>Vukû‘-ı husûf-ı kamer, fî 15 C, leyletü’l-isneyn ve küsûf-ı şems, fî 29 C sene 1233,
 yevmü’s-selâse
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234 14 Z </t>
+!!!-1233-15,29-C</t>
+  </si>
+  <si>
+    <t>1234-Z-14</t>
   </si>
   <si>
     <t>Husûf, fî leyle 14 Z, yevmü’l-isneyn, der-şeb, 22 Eylül sene 1234</t>
   </si>
   <si>
-    <t xml:space="preserve">1235 29 Za </t>
+    <t>1235-ZA-29</t>
   </si>
   <si>
     <t xml:space="preserve">Küsûf-ı âfitâb, fî 29 Za sene 1235, yevmü’l-hamîs, fî sâdis ve’l-işrîn-i Ağustos. Vakt-i asrda,
@@ -344,26 +341,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
     <font/>
     <font>
-      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color rgb="FF231F20"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,22 +384,34 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,8 +630,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.63"/>
-    <col customWidth="1" min="2" max="2" width="76.5"/>
+    <col customWidth="1" min="1" max="1" width="61.13"/>
+    <col customWidth="1" min="2" max="2" width="52.63"/>
     <col customWidth="1" min="3" max="3" width="18.25"/>
     <col customWidth="1" min="4" max="4" width="5.0"/>
     <col customWidth="1" min="5" max="5" width="16.63"/>
@@ -630,149 +646,155 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>46.0</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2011.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2">
+        <v>74.0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2011.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1">
-        <v>74.0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
         <v>78.0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>82.0</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
         <v>82.0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2">
         <v>2011.0</v>
       </c>
     </row>
@@ -780,77 +802,77 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
         <v>86.0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
         <v>86.0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2">
         <v>90.0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2">
         <v>2011.0</v>
       </c>
     </row>
@@ -858,25 +880,25 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>136.0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2">
         <v>2011.0</v>
       </c>
     </row>
@@ -884,25 +906,25 @@
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>138.0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2">
         <v>2011.0</v>
       </c>
     </row>
@@ -910,751 +932,511 @@
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>156.0</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
         <v>194.0</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="E13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>198.0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2">
         <v>278.0</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2">
         <v>288.0</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2">
         <v>296.0</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>298.0</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="E18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
         <v>312.0</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="E19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2">
         <v>334.0</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2">
         <v>348.0</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="E21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>386.0</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
         <v>390.0</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="E23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2">
         <v>410.0</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2">
         <v>414.0</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="E25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2">
         <v>164.0</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="E26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2">
         <v>170.0</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="E27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2">
         <v>348.0</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2">
         <v>374.0</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="E29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="2">
         <v>2011.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
         <v>386.0</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H43" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="1">
-        <v>2011.0</v>
-      </c>
-    </row>
+      <c r="E30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2011.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1"/>
     <row r="48" ht="15.75" customHeight="1"/>

</xml_diff>